<commit_message>
last fix I hope
</commit_message>
<xml_diff>
--- a/lab1.05/lab1.05.xlsx
+++ b/lab1.05/lab1.05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\only_labs_java\physics\lab1.05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99394235-6CD9-4BE8-807F-C096DC46EE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95105BA0-8937-4CFF-B037-723CA94CBD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2953,8 +2953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26:R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3687,28 +3687,28 @@
         <v>29</v>
       </c>
       <c r="M26" s="2">
-        <f>(M24)/($U$16)</f>
-        <v>0.6415641300459155</v>
+        <f>(M24)/(2*0.408*0.06)</f>
+        <v>0.65165702614379084</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" ref="N26:R26" si="8">(N24)/($U$16)</f>
-        <v>0.71499231304131561</v>
+        <f t="shared" ref="N26:R26" si="8">(N24)/(2*0.408*0.06)</f>
+        <v>0.72624035947712418</v>
       </c>
       <c r="O26" s="2">
         <f t="shared" si="8"/>
-        <v>0.80893116167788903</v>
+        <v>0.82165702614379088</v>
       </c>
       <c r="P26" s="2">
         <f t="shared" si="8"/>
-        <v>0.92338067595563555</v>
+        <v>0.93790702614379085</v>
       </c>
       <c r="Q26" s="2">
         <f t="shared" si="8"/>
-        <v>1.0583408558745553</v>
+        <v>1.074990359477124</v>
       </c>
       <c r="R26" s="2">
         <f t="shared" si="8"/>
-        <v>1.2138117014346481</v>
+        <v>1.2329070261437907</v>
       </c>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">

</xml_diff>